<commit_message>
BHR-GT description datafile NL
Added first version of Geotechnisch Booronderzoek (BHR-GT) datafile NL
For details, please see the sheet 'toelichting' in the Excel file itself
</commit_message>
<xml_diff>
--- a/Grondwatermonitoringput (GMW)/BROObject - GMW IMBRO datafile NL (v1.x).xlsx
+++ b/Grondwatermonitoringput (GMW)/BROObject - GMW IMBRO datafile NL (v1.x).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://3hydro-my.sharepoint.com/personal/jos_von_asmuth_3hydro_nl/Documents/GitHub/BRO-Spreadsheet-en-tabelformat/GMW/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://3hydro-my.sharepoint.com/personal/jos_von_asmuth_3hydro_nl/Documents/GitHub/QC-Protocol/BRO-Spreadsheet-en-tabelformat/Grondwatermonitoringput (GMW)/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{A1ED2DD1-39A5-4646-9597-FFCAD7CA7286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A20DA7C4-8EAB-4839-8302-EE0784B6C32D}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26814B37-6F38-4D5A-99CF-A0A5CD7480CB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{26814B37-6F38-4D5A-99CF-A0A5CD7480CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Toelichting" sheetId="8" r:id="rId1"/>
@@ -1378,9 +1378,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1418,7 +1418,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1524,7 +1524,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1666,7 +1666,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1679,7 +1679,7 @@
   </sheetPr>
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1877,8 +1877,8 @@
   </sheetPr>
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>